<commit_message>
fill the excel sheet
</commit_message>
<xml_diff>
--- a/RMS.xlsx
+++ b/RMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -24,19 +24,100 @@
     <t>State</t>
   </si>
   <si>
-    <t xml:space="preserve">     Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     UserStory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Story Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    Comments</t>
-  </si>
-  <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>22-09-14</t>
+  </si>
+  <si>
+    <t>16-09-14</t>
+  </si>
+  <si>
+    <t>thinking of database design</t>
+  </si>
+  <si>
+    <t>wip</t>
+  </si>
+  <si>
+    <t>Shilpa</t>
+  </si>
+  <si>
+    <t>17-09-14</t>
+  </si>
+  <si>
+    <t>designing of tables</t>
+  </si>
+  <si>
+    <t>shilpa</t>
+  </si>
+  <si>
+    <t>cmt</t>
+  </si>
+  <si>
+    <t>18-09-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joining of tables with foreign </t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>19-09-14</t>
+  </si>
+  <si>
+    <t>database diagrams</t>
+  </si>
+  <si>
+    <t>architecture of web application and</t>
+  </si>
+  <si>
+    <t>ashutosh and shilpa</t>
+  </si>
+  <si>
+    <t>23-09-14</t>
+  </si>
+  <si>
+    <t>classes of tables are made in</t>
+  </si>
+  <si>
+    <t>the layer</t>
+  </si>
+  <si>
+    <t>24-09-14</t>
+  </si>
+  <si>
+    <t>designing of login page</t>
+  </si>
+  <si>
+    <t>Ashutosh and shilpa</t>
+  </si>
+  <si>
+    <t>25-09-14</t>
+  </si>
+  <si>
+    <t>design the logo and paste</t>
+  </si>
+  <si>
+    <t>change the color of buttons</t>
+  </si>
+  <si>
+    <t>logo allignment is still left</t>
+  </si>
+  <si>
+    <t>designing of logo is still left</t>
   </si>
 </sst>
 </file>
@@ -375,18 +456,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -394,13 +478,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -410,6 +494,187 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote a code in RMS Dataaccess layer
Made a class LoginAdapter and made a method in that class named
ValidateUser and wrote a code for checking the  login username and
password
</commit_message>
<xml_diff>
--- a/RMS.xlsx
+++ b/RMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>designing of logo is still left</t>
+  </si>
+  <si>
+    <t>26-09-14</t>
+  </si>
+  <si>
+    <t>study and done implementati-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on of stored procedure and </t>
+  </si>
+  <si>
+    <t>made a class in business layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coding on the reset and login click is still left </t>
+  </si>
+  <si>
+    <t>will make a class in data acess layer and connect it with the  web page</t>
   </si>
 </sst>
 </file>
@@ -456,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +488,7 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -675,6 +693,42 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coding for location and area text box are done
area and location textbox retrieve data from the database
</commit_message>
<xml_diff>
--- a/RMS.xlsx
+++ b/RMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -136,12 +136,42 @@
   </si>
   <si>
     <t>will make a class in data acess layer and connect it with the  web page</t>
+  </si>
+  <si>
+    <t>29-09-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code for checking of correct </t>
+  </si>
+  <si>
+    <t>user with correct password is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> done through a database</t>
+  </si>
+  <si>
+    <t>30-09-14</t>
+  </si>
+  <si>
+    <t>designing of a master page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> with a bar and a footer</t>
+  </si>
+  <si>
+    <t>designing of aowner page usi-</t>
+  </si>
+  <si>
+    <t>ng a master page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,8 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +550,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
@@ -538,7 +570,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -558,7 +590,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
@@ -575,6 +607,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -583,7 +616,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -603,7 +636,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
@@ -623,7 +656,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
@@ -640,6 +673,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>25</v>
       </c>
@@ -648,7 +682,7 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="s">
@@ -671,7 +705,7 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
@@ -691,6 +725,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
       <c r="C12" t="s">
         <v>31</v>
       </c>
@@ -699,7 +734,7 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
@@ -719,6 +754,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>36</v>
       </c>
@@ -727,12 +763,104 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>41913</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41680</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
data insertion in database table
</commit_message>
<xml_diff>
--- a/RMS.xlsx
+++ b/RMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -159,10 +159,58 @@
     <t xml:space="preserve"> with a bar and a footer</t>
   </si>
   <si>
-    <t>designing of aowner page usi-</t>
-  </si>
-  <si>
     <t>ng a master page</t>
+  </si>
+  <si>
+    <t>designing of welcome page usi-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designing of a welcome page </t>
+  </si>
+  <si>
+    <t>using a master page</t>
+  </si>
+  <si>
+    <t>create a dropdown toggle on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the navbar named Admin and </t>
+  </si>
+  <si>
+    <t>onclick of that admin dropdow</t>
+  </si>
+  <si>
+    <t>n owner page is opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create two buttons on the </t>
+  </si>
+  <si>
+    <t>ownerpage named property</t>
+  </si>
+  <si>
+    <t>and owner ,which will open</t>
+  </si>
+  <si>
+    <t>a popup when clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modal is not working so proper designing of that age using tabs </t>
+  </si>
+  <si>
+    <t>is still left</t>
+  </si>
+  <si>
+    <t>binding of data in dropdown</t>
+  </si>
+  <si>
+    <t>from database and all the data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is inserted in to the table in </t>
+  </si>
+  <si>
+    <t>database on savechanges click</t>
   </si>
 </sst>
 </file>
@@ -170,7 +218,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -201,10 +249,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,19 +837,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -820,20 +869,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>41913</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -845,17 +894,180 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
       <c r="B23" s="1">
         <v>41680</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41708</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41800</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1">
+        <v>41830</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1">
+        <v>41861</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel sheet filled and changes in owner button click
modal is removed from the Owner button
</commit_message>
<xml_diff>
--- a/RMS.xlsx
+++ b/RMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>database on savechanges click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and same will be done with </t>
+  </si>
+  <si>
+    <t>owner click</t>
+  </si>
+  <si>
+    <t>Owner Details,form Location using tab,Grid showof Form Details</t>
+  </si>
+  <si>
+    <t>Register User,Login Ticket,Password encoding,busy symbol</t>
   </si>
 </sst>
 </file>
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>16</v>
       </c>
@@ -1020,22 +1032,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>17</v>
       </c>
@@ -1055,19 +1067,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>